<commit_message>
Added: get calendar friendly text
</commit_message>
<xml_diff>
--- a/ChurchManager.DataImporter/churchmanager_db_data_import_updated.xlsx
+++ b/ChurchManager.DataImporter/churchmanager_db_data_import_updated.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dilla\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Freelance\ChurchManager\ChurchManager.DataImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91845ADE-FAA1-4D1B-8BCA-649D52994C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A42D892-959C-4FE7-836A-043227351FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="624" windowWidth="26208" windowHeight="16656" tabRatio="357" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="24" windowWidth="26208" windowHeight="16656" tabRatio="357" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Churches" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="People" sheetId="4" r:id="rId4"/>
     <sheet name="HowTo" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1695" uniqueCount="586">
   <si>
     <t>Name*</t>
   </si>
@@ -1798,6 +1798,12 @@
   </si>
   <si>
     <t>Ngobeni Family</t>
+  </si>
+  <si>
+    <t>UserRoles</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -2562,7 +2568,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2619,8 +2625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2680,7 +2686,7 @@
       </c>
       <c r="E2" s="73"/>
       <c r="F2" s="73" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G2" s="73">
         <v>43831</v>
@@ -2706,7 +2712,7 @@
       </c>
       <c r="E3" s="63"/>
       <c r="F3" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G3" s="63">
         <v>43252</v>
@@ -2734,7 +2740,7 @@
         <v>20</v>
       </c>
       <c r="F4" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G4" s="63">
         <v>44166</v>
@@ -2760,7 +2766,7 @@
       </c>
       <c r="E5" s="63"/>
       <c r="F5" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G5" s="63">
         <v>43647</v>
@@ -2788,7 +2794,7 @@
         <v>413</v>
       </c>
       <c r="F6" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G6" s="63">
         <v>43647</v>
@@ -2814,7 +2820,7 @@
       </c>
       <c r="E7" s="63"/>
       <c r="F7" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G7" s="63">
         <v>43435</v>
@@ -2840,7 +2846,7 @@
       </c>
       <c r="E8" s="63"/>
       <c r="F8" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G8" s="63">
         <v>43617</v>
@@ -2866,7 +2872,7 @@
       </c>
       <c r="E9" s="63"/>
       <c r="F9" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G9" s="63">
         <v>43770</v>
@@ -2892,7 +2898,7 @@
       </c>
       <c r="E10" s="63"/>
       <c r="F10" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G10" s="63">
         <v>43739</v>
@@ -2918,7 +2924,7 @@
       </c>
       <c r="E11" s="63"/>
       <c r="F11" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G11" s="63">
         <v>43739</v>
@@ -2946,7 +2952,7 @@
         <v>424</v>
       </c>
       <c r="F12" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G12" s="63">
         <v>43739</v>
@@ -2974,7 +2980,7 @@
         <v>32</v>
       </c>
       <c r="F13" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G13" s="63">
         <v>43556</v>
@@ -3000,7 +3006,7 @@
       </c>
       <c r="E14" s="63"/>
       <c r="F14" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G14" s="63">
         <v>43739</v>
@@ -3028,7 +3034,7 @@
         <v>32</v>
       </c>
       <c r="F15" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G15" s="63">
         <v>44105</v>
@@ -3054,7 +3060,7 @@
       </c>
       <c r="E16" s="63"/>
       <c r="F16" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G16" s="63">
         <v>44256</v>
@@ -3080,7 +3086,7 @@
       </c>
       <c r="E17" s="63"/>
       <c r="F17" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G17" s="63">
         <v>44256</v>
@@ -3106,7 +3112,7 @@
       </c>
       <c r="E18" s="63"/>
       <c r="F18" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G18" s="63">
         <v>42064</v>
@@ -3134,7 +3140,7 @@
         <v>20</v>
       </c>
       <c r="F19" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G19" s="63">
         <v>44166</v>
@@ -3160,7 +3166,7 @@
       </c>
       <c r="E20" s="63"/>
       <c r="F20" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G20" s="63">
         <v>41640</v>
@@ -3186,7 +3192,7 @@
       </c>
       <c r="E21" s="63"/>
       <c r="F21" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G21" s="63">
         <v>42430</v>
@@ -3212,7 +3218,7 @@
       </c>
       <c r="E22" s="63"/>
       <c r="F22" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G22" s="63">
         <v>42430</v>
@@ -3238,7 +3244,7 @@
       </c>
       <c r="E23" s="63"/>
       <c r="F23" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G23" s="63">
         <v>43405</v>
@@ -3264,7 +3270,7 @@
       </c>
       <c r="E24" s="63"/>
       <c r="F24" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G24" s="63">
         <v>41122</v>
@@ -3290,7 +3296,7 @@
       </c>
       <c r="E25" s="63"/>
       <c r="F25" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G25" s="63">
         <v>39814</v>
@@ -3316,7 +3322,7 @@
       </c>
       <c r="E26" s="63"/>
       <c r="F26" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G26" s="63">
         <v>43525</v>
@@ -3342,7 +3348,7 @@
       </c>
       <c r="E27" s="63"/>
       <c r="F27" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G27" s="63">
         <v>40603</v>
@@ -3368,7 +3374,7 @@
       </c>
       <c r="E28" s="63"/>
       <c r="F28" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G28" s="63">
         <v>43374</v>
@@ -3394,7 +3400,7 @@
       </c>
       <c r="E29" s="63"/>
       <c r="F29" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G29" s="63">
         <v>40603</v>
@@ -3420,7 +3426,7 @@
       </c>
       <c r="E30" s="63"/>
       <c r="F30" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G30" s="63">
         <v>43862</v>
@@ -3446,7 +3452,7 @@
       </c>
       <c r="E31" s="63"/>
       <c r="F31" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G31" s="63">
         <v>43862</v>
@@ -3472,7 +3478,7 @@
       </c>
       <c r="E32" s="63"/>
       <c r="F32" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G32" s="63">
         <v>41883</v>
@@ -3498,7 +3504,7 @@
       </c>
       <c r="E33" s="63"/>
       <c r="F33" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G33" s="63">
         <v>43586</v>
@@ -3524,7 +3530,7 @@
       </c>
       <c r="E34" s="63"/>
       <c r="F34" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G34" s="63">
         <v>43101</v>
@@ -3550,7 +3556,7 @@
       </c>
       <c r="E35" s="63"/>
       <c r="F35" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G35" s="63">
         <v>43525</v>
@@ -3576,7 +3582,7 @@
       </c>
       <c r="E36" s="63"/>
       <c r="F36" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G36" s="63">
         <v>42795</v>
@@ -3602,7 +3608,7 @@
       </c>
       <c r="E37" s="63"/>
       <c r="F37" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G37" s="63">
         <v>43160</v>
@@ -3628,7 +3634,7 @@
       </c>
       <c r="E38" s="63"/>
       <c r="F38" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G38" s="63">
         <v>44197</v>
@@ -3654,7 +3660,7 @@
       </c>
       <c r="E39" s="63"/>
       <c r="F39" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G39" s="63">
         <v>44317</v>
@@ -3680,7 +3686,7 @@
       </c>
       <c r="E40" s="63"/>
       <c r="F40" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G40" s="63">
         <v>44317</v>
@@ -3708,7 +3714,7 @@
         <v>55</v>
       </c>
       <c r="F41" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G41" s="63">
         <v>44287</v>
@@ -3736,7 +3742,7 @@
         <v>413</v>
       </c>
       <c r="F42" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G42" s="63">
         <v>44287</v>
@@ -3762,7 +3768,7 @@
       </c>
       <c r="E43" s="63"/>
       <c r="F43" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G43" s="63">
         <v>44287</v>
@@ -3788,7 +3794,7 @@
       </c>
       <c r="E44" s="63"/>
       <c r="F44" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G44" s="63">
         <v>44256</v>
@@ -3814,7 +3820,7 @@
       </c>
       <c r="E45" s="63"/>
       <c r="F45" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G45" s="63">
         <v>44287</v>
@@ -3842,7 +3848,7 @@
         <v>425</v>
       </c>
       <c r="F46" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G46" s="63">
         <v>44317</v>
@@ -3870,7 +3876,7 @@
         <v>425</v>
       </c>
       <c r="F47" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G47" s="63">
         <v>44317</v>
@@ -3898,7 +3904,7 @@
         <v>426</v>
       </c>
       <c r="F48" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G48" s="63">
         <v>44287</v>
@@ -3926,7 +3932,7 @@
         <v>426</v>
       </c>
       <c r="F49" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G49" s="63">
         <v>44287</v>
@@ -3952,7 +3958,7 @@
       </c>
       <c r="E50" s="63"/>
       <c r="F50" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G50" s="63">
         <v>44317</v>
@@ -3980,7 +3986,7 @@
         <v>55</v>
       </c>
       <c r="F51" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G51" s="63">
         <v>44317</v>
@@ -4006,7 +4012,7 @@
       </c>
       <c r="E52" s="63"/>
       <c r="F52" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G52" s="63">
         <v>44256</v>
@@ -4034,7 +4040,7 @@
         <v>426</v>
       </c>
       <c r="F53" s="63" t="s">
-        <v>5</v>
+        <v>444</v>
       </c>
       <c r="G53" s="63">
         <v>44287</v>
@@ -4105,7 +4111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
@@ -5071,10 +5077,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AE76"/>
+  <dimension ref="A1:AF76"/>
   <sheetViews>
-    <sheetView topLeftCell="V2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AC20" sqref="AC20"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AI45" sqref="AI45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5108,10 +5114,11 @@
     <col min="29" max="29" width="53.77734375" style="66" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="46.77734375" bestFit="1" customWidth="1"/>
-    <col min="32" max="1024" width="8.5546875" customWidth="1"/>
+    <col min="32" max="32" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="1024" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>92</v>
       </c>
@@ -5205,8 +5212,11 @@
       <c r="AE1" s="68" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" s="76" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF1" s="68" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" s="76" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="73" t="s">
         <v>85</v>
       </c>
@@ -5290,8 +5300,11 @@
       <c r="AE2" s="73" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" s="76" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF2" s="73" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" s="76" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="73" t="s">
         <v>85</v>
       </c>
@@ -5371,8 +5384,9 @@
         <v>124</v>
       </c>
       <c r="AE3" s="73"/>
-    </row>
-    <row r="4" spans="1:31" s="76" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF3" s="73"/>
+    </row>
+    <row r="4" spans="1:32" s="76" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="73" t="s">
         <v>85</v>
       </c>
@@ -5436,8 +5450,9 @@
         <v>124</v>
       </c>
       <c r="AE4" s="73"/>
-    </row>
-    <row r="5" spans="1:31" s="76" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF4" s="73"/>
+    </row>
+    <row r="5" spans="1:32" s="76" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="73" t="s">
         <v>85</v>
       </c>
@@ -5499,8 +5514,9 @@
         <v>124</v>
       </c>
       <c r="AE5" s="73"/>
-    </row>
-    <row r="6" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF5" s="73"/>
+    </row>
+    <row r="6" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
         <v>147</v>
       </c>
@@ -5580,8 +5596,9 @@
       <c r="AE6" s="32" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="7" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF6" s="32"/>
+    </row>
+    <row r="7" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="str">
         <f>_xlfn.CONCAT(F7, " Family")</f>
         <v>Gurure Family</v>
@@ -5660,8 +5677,9 @@
       <c r="AE7" s="32" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="8" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF7" s="32"/>
+    </row>
+    <row r="8" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="str">
         <f t="shared" ref="A8:A56" si="0">_xlfn.CONCAT(F8, " Family")</f>
         <v>Phiri Family</v>
@@ -5742,8 +5760,9 @@
       <c r="AE8" s="32" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF8" s="32"/>
+    </row>
+    <row r="9" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Manzana Family</v>
@@ -5824,8 +5843,9 @@
       <c r="AE9" s="32" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF9" s="32"/>
+    </row>
+    <row r="10" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Sombhane Family</v>
@@ -5906,8 +5926,9 @@
       <c r="AE10" s="32" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="11" spans="1:31" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF10" s="32"/>
+    </row>
+    <row r="11" spans="1:32" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Addico Family</v>
@@ -5988,8 +6009,9 @@
       <c r="AE11" s="32" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="12" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF11" s="32"/>
+    </row>
+    <row r="12" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Kapalasa Family</v>
@@ -6070,8 +6092,9 @@
       <c r="AE12" s="32" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF12" s="32"/>
+    </row>
+    <row r="13" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Nqunqa Family</v>
@@ -6150,8 +6173,9 @@
       <c r="AE13" s="32" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="14" spans="1:31" s="61" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AF13" s="32"/>
+    </row>
+    <row r="14" spans="1:32" s="61" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Hiliza Family</v>
@@ -6230,8 +6254,9 @@
       <c r="AE14" s="32" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="15" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF14" s="32"/>
+    </row>
+    <row r="15" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Oketunji Family</v>
@@ -6310,8 +6335,9 @@
       <c r="AE15" s="32" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="16" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF15" s="32"/>
+    </row>
+    <row r="16" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Chianu Family</v>
@@ -6386,8 +6412,9 @@
       <c r="AE16" s="32" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="17" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF16" s="32"/>
+    </row>
+    <row r="17" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Mgayi Family</v>
@@ -6468,8 +6495,9 @@
       <c r="AE17" s="32" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="18" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF17" s="32"/>
+    </row>
+    <row r="18" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Zharare Family</v>
@@ -6550,8 +6578,9 @@
       <c r="AE18" s="32" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="19" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF18" s="32"/>
+    </row>
+    <row r="19" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Zharare Family</v>
@@ -6632,8 +6661,9 @@
       <c r="AE19" s="32" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="20" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF19" s="32"/>
+    </row>
+    <row r="20" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Awasi Family</v>
@@ -6712,8 +6742,9 @@
       <c r="AE20" s="32" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="21" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF20" s="32"/>
+    </row>
+    <row r="21" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Makombe Family</v>
@@ -6794,8 +6825,9 @@
       <c r="AE21" s="32" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="22" spans="1:31" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="AF21" s="32"/>
+    </row>
+    <row r="22" spans="1:32" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A22" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Negomo Family</v>
@@ -6876,8 +6908,9 @@
       <c r="AE22" s="32" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="23" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF22" s="32"/>
+    </row>
+    <row r="23" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Rugara Family</v>
@@ -6954,8 +6987,9 @@
       <c r="AE23" s="32" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="24" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF23" s="32"/>
+    </row>
+    <row r="24" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Manyengawana Family</v>
@@ -7036,8 +7070,9 @@
       <c r="AE24" s="32" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="25" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF24" s="32"/>
+    </row>
+    <row r="25" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Goneso  Family</v>
@@ -7116,8 +7151,9 @@
       <c r="AE25" s="32" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="26" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF25" s="32"/>
+    </row>
+    <row r="26" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Olu-Ojo Family</v>
@@ -7198,8 +7234,9 @@
       <c r="AE26" s="32" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="27" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF26" s="32"/>
+    </row>
+    <row r="27" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Siganga Family</v>
@@ -7278,8 +7315,9 @@
       <c r="AE27" s="32" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="28" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF27" s="32"/>
+    </row>
+    <row r="28" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Ngaba Family</v>
@@ -7358,8 +7396,9 @@
       <c r="AE28" s="32" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="29" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF28" s="32"/>
+    </row>
+    <row r="29" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Mdleleni Family</v>
@@ -7438,8 +7477,9 @@
       <c r="AE29" s="32" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="30" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF29" s="32"/>
+    </row>
+    <row r="30" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Waliva Family</v>
@@ -7520,8 +7560,9 @@
       <c r="AE30" s="32" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="31" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF30" s="32"/>
+    </row>
+    <row r="31" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Schneider  Family</v>
@@ -7602,8 +7643,9 @@
       <c r="AE31" s="32" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="32" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF31" s="32"/>
+    </row>
+    <row r="32" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Louise Family</v>
@@ -7680,8 +7722,9 @@
       <c r="AE32" s="32" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="33" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF32" s="32"/>
+    </row>
+    <row r="33" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Macaula Family</v>
@@ -7762,8 +7805,9 @@
       <c r="AE33" s="32" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="34" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF33" s="32"/>
+    </row>
+    <row r="34" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Macaula Family</v>
@@ -7844,8 +7888,9 @@
       <c r="AE34" s="32" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="35" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF34" s="32"/>
+    </row>
+    <row r="35" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Mbesane Family</v>
@@ -7926,8 +7971,9 @@
       <c r="AE35" s="32" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="36" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF35" s="32"/>
+    </row>
+    <row r="36" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Muhwati Family</v>
@@ -8008,8 +8054,9 @@
       <c r="AE36" s="32" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="37" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF36" s="32"/>
+    </row>
+    <row r="37" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Mabunda  Family</v>
@@ -8086,8 +8133,9 @@
       <c r="AE37" s="32" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="38" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF37" s="32"/>
+    </row>
+    <row r="38" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Magondi Family</v>
@@ -8168,8 +8216,9 @@
       <c r="AE38" s="32" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="39" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF38" s="32"/>
+    </row>
+    <row r="39" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Makurumidze Family</v>
@@ -8250,8 +8299,9 @@
       <c r="AE39" s="32" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="40" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF39" s="32"/>
+    </row>
+    <row r="40" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Noludwe Family</v>
@@ -8332,8 +8382,9 @@
       <c r="AE40" s="32" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="41" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF40" s="32"/>
+    </row>
+    <row r="41" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Temisan Family</v>
@@ -8410,8 +8461,9 @@
       <c r="AE41" s="32" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="42" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF41" s="32"/>
+    </row>
+    <row r="42" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Nteta Family</v>
@@ -8488,8 +8540,9 @@
       <c r="AE42" s="32" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="43" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF42" s="32"/>
+    </row>
+    <row r="43" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Titus Family</v>
@@ -8570,8 +8623,9 @@
       <c r="AE43" s="32" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="44" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF43" s="32"/>
+    </row>
+    <row r="44" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Galela Family</v>
@@ -8652,8 +8706,9 @@
       <c r="AE44" s="32" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="45" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF44" s="32"/>
+    </row>
+    <row r="45" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Tengani Family</v>
@@ -8734,8 +8789,9 @@
       <c r="AE45" s="32" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="46" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF45" s="32"/>
+    </row>
+    <row r="46" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Chihota Family</v>
@@ -8816,8 +8872,9 @@
       <c r="AE46" s="32" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="47" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF46" s="32"/>
+    </row>
+    <row r="47" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Lesole Family</v>
@@ -8898,8 +8955,9 @@
       <c r="AE47" s="32" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="48" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF47" s="32"/>
+    </row>
+    <row r="48" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Sigenu Family</v>
@@ -8976,8 +9034,9 @@
       <c r="AE48" s="32" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="49" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF48" s="32"/>
+    </row>
+    <row r="49" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Mashandudze Family</v>
@@ -9058,8 +9117,9 @@
       <c r="AE49" s="32" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="50" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF49" s="32"/>
+    </row>
+    <row r="50" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Mashandudze Family</v>
@@ -9140,8 +9200,9 @@
       <c r="AE50" s="32" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="51" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF50" s="32"/>
+    </row>
+    <row r="51" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Ndong Family</v>
@@ -9222,8 +9283,9 @@
       <c r="AE51" s="32" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="52" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF51" s="32"/>
+    </row>
+    <row r="52" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Maraitjies Family</v>
@@ -9304,8 +9366,9 @@
       <c r="AE52" s="32" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="53" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF52" s="32"/>
+    </row>
+    <row r="53" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Ndlovu Family</v>
@@ -9386,8 +9449,9 @@
       <c r="AE53" s="32" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="54" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF53" s="32"/>
+    </row>
+    <row r="54" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Makiwa Family</v>
@@ -9468,8 +9532,9 @@
       <c r="AE54" s="32" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="55" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF54" s="32"/>
+    </row>
+    <row r="55" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Fon Family</v>
@@ -9548,8 +9613,9 @@
       <c r="AE55" s="32" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="56" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF55" s="32"/>
+    </row>
+    <row r="56" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Ngobeni Family</v>
@@ -9630,8 +9696,9 @@
       <c r="AE56" s="32" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AF56" s="32"/>
+    </row>
+    <row r="57" spans="1:32" x14ac:dyDescent="0.3">
       <c r="G57" s="7"/>
       <c r="H57" s="8"/>
       <c r="I57" s="8"/>
@@ -9640,7 +9707,7 @@
       <c r="L57" s="10"/>
       <c r="M57" s="11"/>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:32" x14ac:dyDescent="0.3">
       <c r="G58" s="7"/>
       <c r="H58" s="8"/>
       <c r="I58" s="8"/>
@@ -9649,7 +9716,7 @@
       <c r="L58" s="10"/>
       <c r="M58" s="11"/>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:32" x14ac:dyDescent="0.3">
       <c r="G59" s="7"/>
       <c r="H59" s="8"/>
       <c r="I59" s="8"/>
@@ -9658,7 +9725,7 @@
       <c r="L59" s="10"/>
       <c r="M59" s="11"/>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:32" x14ac:dyDescent="0.3">
       <c r="G60" s="7"/>
       <c r="H60" s="8"/>
       <c r="I60" s="8"/>
@@ -9667,7 +9734,7 @@
       <c r="L60" s="10"/>
       <c r="M60" s="11"/>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:32" x14ac:dyDescent="0.3">
       <c r="G61" s="7"/>
       <c r="H61" s="8"/>
       <c r="I61" s="8"/>
@@ -9679,7 +9746,7 @@
       <c r="T61" s="14"/>
       <c r="U61" s="15"/>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:32" x14ac:dyDescent="0.3">
       <c r="G62" s="7"/>
       <c r="H62" s="8"/>
       <c r="I62" s="8"/>
@@ -9691,7 +9758,7 @@
       <c r="T62" s="14"/>
       <c r="U62" s="15"/>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:32" x14ac:dyDescent="0.3">
       <c r="G63" s="7"/>
       <c r="H63" s="8"/>
       <c r="I63" s="8"/>
@@ -9703,7 +9770,7 @@
       <c r="T63" s="14"/>
       <c r="U63" s="15"/>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:32" x14ac:dyDescent="0.3">
       <c r="G64" s="7"/>
       <c r="H64" s="8"/>
       <c r="I64" s="8"/>

</xml_diff>